<commit_message>
Changed to 24 MHz oscillator
EC mode should be bettter based on errata.
</commit_message>
<xml_diff>
--- a/Schematic/RX12-BOM.xlsx
+++ b/Schematic/RX12-BOM.xlsx
@@ -37,9 +37,6 @@
     <t>PIC32, PIC32MKxxxGPD/E064</t>
   </si>
   <si>
-    <t>Xtal, 8 MHz</t>
-  </si>
-  <si>
     <t>CAPACITOR, 27pF</t>
   </si>
   <si>
@@ -130,9 +127,6 @@
     <t>Microchip\TQFP-64(PT)</t>
   </si>
   <si>
-    <t>Ultiboard\Xtal 2-SMD</t>
-  </si>
-  <si>
     <t>Ultiboard\0805LED</t>
   </si>
   <si>
@@ -163,7 +157,13 @@
     <t>455-1670-ND</t>
   </si>
   <si>
-    <t>887-1448-1-ND</t>
+    <t>Xtal, Osc 24 MHz</t>
+  </si>
+  <si>
+    <t>Osc-3225</t>
+  </si>
+  <si>
+    <t>1253-1406-1-ND</t>
   </si>
 </sst>
 </file>
@@ -187,7 +187,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -195,13 +195,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,7 +517,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B9" sqref="B9:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -512,19 +530,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
         <v>42</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>43</v>
       </c>
-      <c r="C1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>45</v>
-      </c>
-      <c r="E1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -532,16 +550,16 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
         <v>46</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -552,10 +570,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -566,10 +584,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -580,10 +598,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -594,10 +612,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -608,10 +626,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -622,26 +640,26 @@
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9">
         <v>1</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="B9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>49</v>
       </c>
     </row>
@@ -650,13 +668,13 @@
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -664,13 +682,13 @@
         <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -678,13 +696,13 @@
         <v>3</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -692,13 +710,13 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -706,13 +724,13 @@
         <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -720,13 +738,13 @@
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -734,13 +752,13 @@
         <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -751,13 +769,16 @@
         <v>0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E9" r:id="rId1" display="http://www.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;itemSeq=190230225&amp;uq=635920776589211423"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed LED resistors to 150 ohm to reduce current
</commit_message>
<xml_diff>
--- a/Schematic/RX12-BOM.xlsx
+++ b/Schematic/RX12-BOM.xlsx
@@ -40,9 +40,6 @@
     <t>LED_green</t>
   </si>
   <si>
-    <t>RESISTOR, 33Ω</t>
-  </si>
-  <si>
     <t>CAPACITOR, 0.1µF</t>
   </si>
   <si>
@@ -152,6 +149,9 @@
   </si>
   <si>
     <t>C3, C4, C5, C6, C7,C8</t>
+  </si>
+  <si>
+    <t>RESISTOR, 150Ω</t>
   </si>
 </sst>
 </file>
@@ -493,7 +493,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -506,19 +506,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
         <v>35</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>36</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>37</v>
       </c>
-      <c r="D1" t="s">
-        <v>38</v>
-      </c>
       <c r="E1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -526,16 +526,16 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -546,10 +546,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -560,10 +560,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -574,10 +574,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -588,10 +588,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -602,10 +602,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -616,10 +616,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -627,16 +627,16 @@
         <v>1</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -647,10 +647,10 @@
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -658,13 +658,13 @@
         <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="28.8">
@@ -672,13 +672,13 @@
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -686,13 +686,13 @@
         <v>2</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -700,13 +700,13 @@
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -717,10 +717,10 @@
         <v>0</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated schematic and BOM to AP2210N regulator.
Also DSC6001 oscillator
</commit_message>
<xml_diff>
--- a/Schematic/RX12-BOM.xlsx
+++ b/Schematic/RX12-BOM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
   <si>
     <t>HEADERS_TEST, HDR1X3</t>
   </si>
@@ -22,12 +22,6 @@
     <t>Headers, HDR3X4</t>
   </si>
   <si>
-    <t>VoltageRegulator, MCP1702-3.3</t>
-  </si>
-  <si>
-    <t>CAPACITOR, 1µF</t>
-  </si>
-  <si>
     <t>CAPACITOR, 10µF</t>
   </si>
   <si>
@@ -145,26 +139,42 @@
     <t>Osc-3225</t>
   </si>
   <si>
-    <t>1253-1406-1-ND</t>
-  </si>
-  <si>
     <t>C3, C4, C5, C6, C7,C8</t>
   </si>
   <si>
     <t>RESISTOR, 150Ω</t>
+  </si>
+  <si>
+    <t>DSC6001CI2A-024.0000-ND</t>
+  </si>
+  <si>
+    <t>AP2210N-3.3TRG1DICT-ND</t>
+  </si>
+  <si>
+    <t>VoltageRegulator, AP2210N-3.3</t>
+  </si>
+  <si>
+    <t>CAPACITOR, 2.2µF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -184,10 +194,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
@@ -196,8 +210,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -493,7 +509,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -506,19 +522,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>35</v>
       </c>
-      <c r="C1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>37</v>
-      </c>
-      <c r="E1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -526,16 +542,16 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
         <v>38</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -546,10 +562,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -557,13 +573,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -571,13 +590,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -585,13 +604,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -599,13 +618,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -613,13 +632,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -627,15 +646,15 @@
         <v>1</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>43</v>
       </c>
     </row>
@@ -644,13 +663,13 @@
         <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -658,13 +677,13 @@
         <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="28.8">
@@ -672,13 +691,13 @@
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -686,13 +705,13 @@
         <v>2</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -700,13 +719,13 @@
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -717,17 +736,18 @@
         <v>0</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E9" r:id="rId1" display="http://www.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;itemSeq=190230225&amp;uq=635920776589211423"/>
+    <hyperlink ref="E9" r:id="rId1" display="https://www.digikey.com/product-detail/en/microchip-technology/DSC6001CI2A-024.0000/DSC6001CI2A-024.0000-ND/7732678"/>
+    <hyperlink ref="E4" r:id="rId2" display="https://www.digikey.com/product-detail/en/diodes-incorporated/AP2210N-3.3TRG1/AP2210N-3.3TRG1DICT-ND/4505294"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>